<commit_message>
- modificata la funzione check_art() per la verifica della presenza dell'articolo in MP (check_valori) - aggiunto alla funzione export_file() il caso in cui il file inserito nella combobox non sia presente - modifica dell'interfaccia grafica, sia visiva che funzioni - eliminato save_panel perchè si salva tutto alla chiusura
</commit_message>
<xml_diff>
--- a/AppInventario/files/inventario3.xlsx
+++ b/AppInventario/files/inventario3.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -440,17 +440,17 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>100</v>
+        <v>500</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>00010012</t>
+          <t>90351051</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>500</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4">
@@ -460,16 +460,6 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>90351051</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
         <v>1000</v>
       </c>
     </row>

</xml_diff>